<commit_message>
Deploying to gh-pages from @ IDGRLP/Tumorkonferenzen-IG@eaacc36b41e96a8294167bdcaa7ea403bea3fa83 🚀
</commit_message>
<xml_diff>
--- a/StructureDefinition-TumorPatient.xlsx
+++ b/StructureDefinition-TumorPatient.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3230" uniqueCount="630">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3230" uniqueCount="624">
   <si>
     <t>Property</t>
   </si>
@@ -60,7 +60,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-12-02T15:35:52+00:00</t>
+    <t>2025-02-09T15:43:55+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -515,9 +515,6 @@
   </si>
   <si>
     <t>Krankenversichertennummer</t>
-  </si>
-  <si>
-    <t>An identifier - identifies some entity uniquely and unambiguously. Typically this is used for business identifiers.</t>
   </si>
   <si>
     <t>&lt;valueIdentifier xmlns="http://hl7.org/fhir"&gt;
@@ -530,16 +527,6 @@
 &lt;/valueIdentifier&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">ele-1
-</t>
-  </si>
-  <si>
-    <t>II - The Identifier class is a little looser than the v3 type II because it allows URIs as well as registered OIDs or GUIDs.  Also maps to Role[classCode=IDENT]</t>
-  </si>
-  <si>
-    <t>CX / EI (occasionally, more often EI maps to a resource id or a URL)</t>
-  </si>
-  <si>
     <t>Patient.identifier:krankenversichertennummer.id</t>
   </si>
   <si>
@@ -1146,37 +1133,25 @@
 </t>
   </si>
   <si>
-    <t>Eine Adresse gemäß postalischer Konventionen</t>
-  </si>
-  <si>
-    <t>Eine Adresse gemäß postalischer Konventionen (im Gegensatz zu bspw. GPS-Koordinaten). Die Adresse kann sowohl zur Zustellung von Postsendungen oder zum Aufsuchen von Orten, die keine gültige Postadresse haben, verwendet werden.
-Die verwendeten Extensions in diesem Profil bilden die Struktur der Adresse ab, wie sie im VSDM-Format der elektronischen Versichertenkarte verwendet wird.
-Insbesondere bei ausländischen Adresse oder Adressen, die nicht durch Einlesen einer elektronischen Versichertenkarte erfasst wurden, sind abweichende Strukturen möglich. Die Verwendung der Extensions ist nicht verpflichtend.</t>
-  </si>
-  <si>
-    <t>Note: address is intended to describe postal addresses for administrative purposes, not to describe absolute geographical coordinates.  Postal addresses are often used as proxies for physical locations (also see the [Location](http://hl7.org/fhir/R4/location.html#) resource).</t>
+    <t>An address for the individual</t>
+  </si>
+  <si>
+    <t>An address for the individual.</t>
+  </si>
+  <si>
+    <t>Patient may have multiple addresses with different uses or applicable periods.</t>
   </si>
   <si>
     <t>May need to keep track of patient addresses for contacting, billing or reporting requirements and also to help with identification.</t>
   </si>
   <si>
-    <t>&lt;valueAddress xmlns="http://hl7.org/fhir"&gt;
-  &lt;use value="home"/&gt;
-  &lt;type value="postal"/&gt;
-  &lt;line value="Musterweg 42"/&gt;
-  &lt;city value="Musterhausen"/&gt;
-  &lt;postalCode value="99999"/&gt;
-&lt;/valueAddress&gt;</t>
-  </si>
-  <si>
-    <t>ele-1:All FHIR elements must have a @value or children {hasValue() or (children().count() &gt; id.count())}
-add-1:Wenn die Extension 'Hausnummer' verwendet wird, muss auch Address.line gefüllt werden {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-houseNumber').empty() or $this.hasValue())}add-2:Wenn die Extension 'Strasse' verwendet wird, muss auch Address.line gefüllt werden {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-streetName').empty() or $this.hasValue())}add-3:Wenn die Extension 'Postfach' verwendet wird, muss auch Address.line gefüllt werden {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-postBox').empty() or $this.hasValue())}add-4:Eine Postfach-Adresse darf nicht vom Type "physical" oder "both" sein. {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-postBox').empty() or $this.hasValue()) or type='postal' or type.empty()}add-5:Wenn die Extension 'Adresszusatz' verwendet wird, muss auch Address.line gefüllt werden {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-additionalLocator').empty() or $this.hasValue())}add-6:Wenn die Extension 'Postfach' verwendet wird, dürfen die Extensions 'Strasse' und 'Hausnummer' nicht verwendet werden {line.all($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-postBox').empty() or ($this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-streetName').empty() and $this.extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-houseNumber').empty()))}add-7:Wenn die Extension 'Precinct' (Stadtteil) verwendet wird, dann muss diese Information auch als separates line-item abgebildet sein. {extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-precinct').empty() or all(line contains extension('http://hl7.org/fhir/StructureDefinition/iso21090-ADXP-precinct').value.ofType(string))}</t>
-  </si>
-  <si>
-    <t>AD</t>
-  </si>
-  <si>
-    <t>XAD</t>
+    <t>addr</t>
+  </si>
+  <si>
+    <t>.addr</t>
+  </si>
+  <si>
+    <t>PID-11</t>
   </si>
   <si>
     <t>Patient.address.id</t>
@@ -1761,9 +1736,6 @@
   </si>
   <si>
     <t>Need to keep track where the contact person can be contacted per postal mail or visited.</t>
-  </si>
-  <si>
-    <t>addr</t>
   </si>
   <si>
     <t>NK1-4</t>
@@ -2350,7 +2322,7 @@
     <col min="17" max="17" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="18" max="18" width="20.703125" customWidth="true" bestFit="true"/>
     <col min="19" max="19" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="20" max="20" width="41.56640625" customWidth="true" bestFit="true"/>
+    <col min="20" max="20" width="39.97265625" customWidth="true" bestFit="true"/>
     <col min="21" max="21" width="17.171875" customWidth="true" bestFit="true"/>
     <col min="22" max="22" width="17.65625" customWidth="true" bestFit="true"/>
     <col min="23" max="23" width="19.03515625" customWidth="true" bestFit="true"/>
@@ -3691,7 +3663,7 @@
         <v>20</v>
       </c>
       <c r="J12" t="s" s="2">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="K12" t="s" s="2">
         <v>158</v>
@@ -3700,7 +3672,7 @@
         <v>159</v>
       </c>
       <c r="M12" t="s" s="2">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="N12" s="2"/>
       <c r="O12" t="s" s="2">
@@ -3714,7 +3686,7 @@
         <v>20</v>
       </c>
       <c r="S12" t="s" s="2">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="T12" t="s" s="2">
         <v>20</v>
@@ -3762,22 +3734,22 @@
         <v>80</v>
       </c>
       <c r="AI12" t="s" s="2">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="AJ12" t="s" s="2">
         <v>100</v>
       </c>
       <c r="AK12" t="s" s="2">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="AL12" t="s" s="2">
-        <v>20</v>
+        <v>153</v>
       </c>
       <c r="AM12" t="s" s="2">
-        <v>20</v>
+        <v>154</v>
       </c>
       <c r="AN12" t="s" s="2">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="AO12" t="s" s="2">
         <v>20</v>
@@ -3785,10 +3757,10 @@
     </row>
     <row r="13" hidden="true">
       <c r="A13" t="s" s="2">
-        <v>165</v>
+        <v>161</v>
       </c>
       <c r="B13" t="s" s="2">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="C13" s="2"/>
       <c r="D13" t="s" s="2">
@@ -3811,13 +3783,13 @@
         <v>20</v>
       </c>
       <c r="K13" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L13" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M13" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N13" s="2"/>
       <c r="O13" s="2"/>
@@ -3868,7 +3840,7 @@
         <v>20</v>
       </c>
       <c r="AF13" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG13" t="s" s="2">
         <v>79</v>
@@ -3883,7 +3855,7 @@
         <v>20</v>
       </c>
       <c r="AK13" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL13" t="s" s="2">
         <v>20</v>
@@ -3900,10 +3872,10 @@
     </row>
     <row r="14" hidden="true">
       <c r="A14" t="s" s="2">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="B14" t="s" s="2">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" t="s" s="2">
@@ -3932,7 +3904,7 @@
         <v>135</v>
       </c>
       <c r="M14" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N14" t="s" s="2">
         <v>137</v>
@@ -3973,10 +3945,10 @@
         <v>20</v>
       </c>
       <c r="AB14" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AC14" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AD14" t="s" s="2">
         <v>20</v>
@@ -3985,7 +3957,7 @@
         <v>151</v>
       </c>
       <c r="AF14" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG14" t="s" s="2">
         <v>79</v>
@@ -4000,7 +3972,7 @@
         <v>139</v>
       </c>
       <c r="AK14" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL14" t="s" s="2">
         <v>20</v>
@@ -4017,10 +3989,10 @@
     </row>
     <row r="15" hidden="true">
       <c r="A15" t="s" s="2">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="B15" t="s" s="2">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C15" s="2"/>
       <c r="D15" t="s" s="2">
@@ -4046,16 +4018,16 @@
         <v>108</v>
       </c>
       <c r="L15" t="s" s="2">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="M15" t="s" s="2">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="N15" t="s" s="2">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="O15" t="s" s="2">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="P15" t="s" s="2">
         <v>20</v>
@@ -4080,13 +4052,13 @@
         <v>20</v>
       </c>
       <c r="X15" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y15" t="s" s="2">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="Z15" t="s" s="2">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AA15" t="s" s="2">
         <v>20</v>
@@ -4104,7 +4076,7 @@
         <v>20</v>
       </c>
       <c r="AF15" t="s" s="2">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="AG15" t="s" s="2">
         <v>79</v>
@@ -4119,7 +4091,7 @@
         <v>100</v>
       </c>
       <c r="AK15" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AL15" t="s" s="2">
         <v>20</v>
@@ -4136,10 +4108,10 @@
     </row>
     <row r="16" hidden="true">
       <c r="A16" t="s" s="2">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="B16" t="s" s="2">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="C16" s="2"/>
       <c r="D16" t="s" s="2">
@@ -4162,19 +4134,19 @@
         <v>89</v>
       </c>
       <c r="K16" t="s" s="2">
+        <v>187</v>
+      </c>
+      <c r="L16" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="M16" t="s" s="2">
+        <v>189</v>
+      </c>
+      <c r="N16" t="s" s="2">
+        <v>190</v>
+      </c>
+      <c r="O16" t="s" s="2">
         <v>191</v>
-      </c>
-      <c r="L16" t="s" s="2">
-        <v>192</v>
-      </c>
-      <c r="M16" t="s" s="2">
-        <v>193</v>
-      </c>
-      <c r="N16" t="s" s="2">
-        <v>194</v>
-      </c>
-      <c r="O16" t="s" s="2">
-        <v>195</v>
       </c>
       <c r="P16" t="s" s="2">
         <v>20</v>
@@ -4184,7 +4156,7 @@
         <v>20</v>
       </c>
       <c r="S16" t="s" s="2">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="T16" t="s" s="2">
         <v>20</v>
@@ -4199,11 +4171,11 @@
         <v>20</v>
       </c>
       <c r="X16" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Y16" s="2"/>
       <c r="Z16" t="s" s="2">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="AA16" t="s" s="2">
         <v>20</v>
@@ -4221,7 +4193,7 @@
         <v>20</v>
       </c>
       <c r="AF16" t="s" s="2">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="AG16" t="s" s="2">
         <v>79</v>
@@ -4233,10 +4205,10 @@
         <v>20</v>
       </c>
       <c r="AJ16" t="s" s="2">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="AK16" t="s" s="2">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="AL16" t="s" s="2">
         <v>20</v>
@@ -4245,7 +4217,7 @@
         <v>20</v>
       </c>
       <c r="AN16" t="s" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="AO16" t="s" s="2">
         <v>20</v>
@@ -4253,10 +4225,10 @@
     </row>
     <row r="17" hidden="true">
       <c r="A17" t="s" s="2">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="B17" t="s" s="2">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C17" s="2"/>
       <c r="D17" t="s" s="2">
@@ -4282,29 +4254,29 @@
         <v>102</v>
       </c>
       <c r="L17" t="s" s="2">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="M17" t="s" s="2">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="N17" t="s" s="2">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="O17" t="s" s="2">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="P17" t="s" s="2">
         <v>20</v>
       </c>
       <c r="Q17" s="2"/>
       <c r="R17" t="s" s="2">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="S17" t="s" s="2">
         <v>20</v>
       </c>
       <c r="T17" t="s" s="2">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="U17" t="s" s="2">
         <v>20</v>
@@ -4340,7 +4312,7 @@
         <v>20</v>
       </c>
       <c r="AF17" t="s" s="2">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="AG17" t="s" s="2">
         <v>79</v>
@@ -4355,7 +4327,7 @@
         <v>100</v>
       </c>
       <c r="AK17" t="s" s="2">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="AL17" t="s" s="2">
         <v>20</v>
@@ -4364,7 +4336,7 @@
         <v>20</v>
       </c>
       <c r="AN17" t="s" s="2">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="AO17" t="s" s="2">
         <v>20</v>
@@ -4372,10 +4344,10 @@
     </row>
     <row r="18" hidden="true">
       <c r="A18" t="s" s="2">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="B18" t="s" s="2">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C18" s="2"/>
       <c r="D18" t="s" s="2">
@@ -4398,16 +4370,16 @@
         <v>89</v>
       </c>
       <c r="K18" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L18" t="s" s="2">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="M18" t="s" s="2">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="N18" t="s" s="2">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="O18" s="2"/>
       <c r="P18" t="s" s="2">
@@ -4421,7 +4393,7 @@
         <v>20</v>
       </c>
       <c r="T18" t="s" s="2">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="U18" t="s" s="2">
         <v>20</v>
@@ -4457,7 +4429,7 @@
         <v>20</v>
       </c>
       <c r="AF18" t="s" s="2">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="AG18" t="s" s="2">
         <v>79</v>
@@ -4469,10 +4441,10 @@
         <v>20</v>
       </c>
       <c r="AJ18" t="s" s="2">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="AK18" t="s" s="2">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="AL18" t="s" s="2">
         <v>20</v>
@@ -4481,7 +4453,7 @@
         <v>20</v>
       </c>
       <c r="AN18" t="s" s="2">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="AO18" t="s" s="2">
         <v>20</v>
@@ -4489,10 +4461,10 @@
     </row>
     <row r="19" hidden="true">
       <c r="A19" t="s" s="2">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B19" t="s" s="2">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C19" s="2"/>
       <c r="D19" t="s" s="2">
@@ -4515,13 +4487,13 @@
         <v>89</v>
       </c>
       <c r="K19" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L19" t="s" s="2">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="M19" t="s" s="2">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="N19" s="2"/>
       <c r="O19" s="2"/>
@@ -4572,7 +4544,7 @@
         <v>20</v>
       </c>
       <c r="AF19" t="s" s="2">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="AG19" t="s" s="2">
         <v>79</v>
@@ -4587,7 +4559,7 @@
         <v>100</v>
       </c>
       <c r="AK19" t="s" s="2">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="AL19" t="s" s="2">
         <v>20</v>
@@ -4596,7 +4568,7 @@
         <v>20</v>
       </c>
       <c r="AN19" t="s" s="2">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="AO19" t="s" s="2">
         <v>20</v>
@@ -4604,10 +4576,10 @@
     </row>
     <row r="20" hidden="true">
       <c r="A20" t="s" s="2">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="B20" t="s" s="2">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C20" s="2"/>
       <c r="D20" t="s" s="2">
@@ -4630,16 +4602,16 @@
         <v>89</v>
       </c>
       <c r="K20" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L20" t="s" s="2">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="M20" t="s" s="2">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="N20" t="s" s="2">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="O20" s="2"/>
       <c r="P20" t="s" s="2">
@@ -4689,7 +4661,7 @@
         <v>20</v>
       </c>
       <c r="AF20" t="s" s="2">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="AG20" t="s" s="2">
         <v>79</v>
@@ -4704,7 +4676,7 @@
         <v>100</v>
       </c>
       <c r="AK20" t="s" s="2">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="AL20" t="s" s="2">
         <v>20</v>
@@ -4713,7 +4685,7 @@
         <v>20</v>
       </c>
       <c r="AN20" t="s" s="2">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="AO20" t="s" s="2">
         <v>20</v>
@@ -4721,10 +4693,10 @@
     </row>
     <row r="21" hidden="true">
       <c r="A21" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="B21" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C21" s="2"/>
       <c r="D21" t="s" s="2">
@@ -4747,26 +4719,26 @@
         <v>89</v>
       </c>
       <c r="K21" t="s" s="2">
+        <v>237</v>
+      </c>
+      <c r="L21" t="s" s="2">
+        <v>238</v>
+      </c>
+      <c r="M21" t="s" s="2">
+        <v>239</v>
+      </c>
+      <c r="N21" t="s" s="2">
+        <v>240</v>
+      </c>
+      <c r="O21" t="s" s="2">
         <v>241</v>
       </c>
-      <c r="L21" t="s" s="2">
+      <c r="P21" t="s" s="2">
+        <v>20</v>
+      </c>
+      <c r="Q21" t="s" s="2">
         <v>242</v>
       </c>
-      <c r="M21" t="s" s="2">
-        <v>243</v>
-      </c>
-      <c r="N21" t="s" s="2">
-        <v>244</v>
-      </c>
-      <c r="O21" t="s" s="2">
-        <v>245</v>
-      </c>
-      <c r="P21" t="s" s="2">
-        <v>20</v>
-      </c>
-      <c r="Q21" t="s" s="2">
-        <v>246</v>
-      </c>
       <c r="R21" t="s" s="2">
         <v>20</v>
       </c>
@@ -4810,7 +4782,7 @@
         <v>20</v>
       </c>
       <c r="AF21" t="s" s="2">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="AG21" t="s" s="2">
         <v>79</v>
@@ -4825,13 +4797,13 @@
         <v>100</v>
       </c>
       <c r="AK21" t="s" s="2">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="AL21" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM21" t="s" s="2">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="AN21" t="s" s="2">
         <v>20</v>
@@ -4842,10 +4814,10 @@
     </row>
     <row r="22" hidden="true">
       <c r="A22" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="B22" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C22" s="2"/>
       <c r="D22" t="s" s="2">
@@ -4868,19 +4840,19 @@
         <v>89</v>
       </c>
       <c r="K22" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="L22" t="s" s="2">
+        <v>247</v>
+      </c>
+      <c r="M22" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="N22" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O22" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="L22" t="s" s="2">
-        <v>251</v>
-      </c>
-      <c r="M22" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N22" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="O22" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="P22" t="s" s="2">
         <v>20</v>
@@ -4927,7 +4899,7 @@
         <v>151</v>
       </c>
       <c r="AF22" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="AG22" t="s" s="2">
         <v>79</v>
@@ -4942,16 +4914,16 @@
         <v>100</v>
       </c>
       <c r="AK22" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AL22" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM22" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN22" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AO22" t="s" s="2">
         <v>20</v>
@@ -4959,10 +4931,10 @@
     </row>
     <row r="23" hidden="true">
       <c r="A23" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="B23" t="s" s="2">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C23" s="2"/>
       <c r="D23" t="s" s="2">
@@ -4985,13 +4957,13 @@
         <v>20</v>
       </c>
       <c r="K23" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L23" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M23" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N23" s="2"/>
       <c r="O23" s="2"/>
@@ -5042,7 +5014,7 @@
         <v>20</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>79</v>
@@ -5057,7 +5029,7 @@
         <v>20</v>
       </c>
       <c r="AK23" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL23" t="s" s="2">
         <v>20</v>
@@ -5074,10 +5046,10 @@
     </row>
     <row r="24" hidden="true">
       <c r="A24" t="s" s="2">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -5106,7 +5078,7 @@
         <v>135</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N24" t="s" s="2">
         <v>137</v>
@@ -5147,10 +5119,10 @@
         <v>20</v>
       </c>
       <c r="AB24" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AC24" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AD24" t="s" s="2">
         <v>20</v>
@@ -5159,7 +5131,7 @@
         <v>151</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>79</v>
@@ -5174,7 +5146,7 @@
         <v>139</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL24" t="s" s="2">
         <v>20</v>
@@ -5191,10 +5163,10 @@
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -5220,16 +5192,16 @@
         <v>108</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="O25" t="s" s="2">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="P25" t="s" s="2">
         <v>20</v>
@@ -5254,13 +5226,13 @@
         <v>20</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="Z25" t="s" s="2">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="AA25" t="s" s="2">
         <v>20</v>
@@ -5278,7 +5250,7 @@
         <v>20</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>79</v>
@@ -5293,7 +5265,7 @@
         <v>100</v>
       </c>
       <c r="AK25" t="s" s="2">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="AL25" t="s" s="2">
         <v>20</v>
@@ -5302,7 +5274,7 @@
         <v>20</v>
       </c>
       <c r="AN25" t="s" s="2">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="AO25" t="s" s="2">
         <v>20</v>
@@ -5310,10 +5282,10 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5336,19 +5308,19 @@
         <v>89</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="O26" t="s" s="2">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P26" t="s" s="2">
         <v>20</v>
@@ -5397,7 +5369,7 @@
         <v>20</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>79</v>
@@ -5412,7 +5384,7 @@
         <v>100</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AL26" t="s" s="2">
         <v>20</v>
@@ -5421,7 +5393,7 @@
         <v>20</v>
       </c>
       <c r="AN26" t="s" s="2">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="AO26" t="s" s="2">
         <v>20</v>
@@ -5429,14 +5401,14 @@
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" t="s" s="2">
@@ -5455,16 +5427,16 @@
         <v>89</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -5514,7 +5486,7 @@
         <v>20</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>79</v>
@@ -5529,7 +5501,7 @@
         <v>100</v>
       </c>
       <c r="AK27" t="s" s="2">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="AL27" t="s" s="2">
         <v>20</v>
@@ -5538,7 +5510,7 @@
         <v>20</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="AO27" t="s" s="2">
         <v>20</v>
@@ -5546,14 +5518,14 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" t="s" s="2">
@@ -5572,16 +5544,16 @@
         <v>89</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5631,7 +5603,7 @@
         <v>20</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
@@ -5646,7 +5618,7 @@
         <v>100</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="AL28" t="s" s="2">
         <v>20</v>
@@ -5655,7 +5627,7 @@
         <v>20</v>
       </c>
       <c r="AN28" t="s" s="2">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="AO28" t="s" s="2">
         <v>20</v>
@@ -5663,10 +5635,10 @@
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5689,13 +5661,13 @@
         <v>89</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="N29" s="2"/>
       <c r="O29" s="2"/>
@@ -5746,7 +5718,7 @@
         <v>20</v>
       </c>
       <c r="AF29" t="s" s="2">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="AG29" t="s" s="2">
         <v>79</v>
@@ -5761,7 +5733,7 @@
         <v>100</v>
       </c>
       <c r="AK29" t="s" s="2">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="AL29" t="s" s="2">
         <v>20</v>
@@ -5770,7 +5742,7 @@
         <v>20</v>
       </c>
       <c r="AN29" t="s" s="2">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="AO29" t="s" s="2">
         <v>20</v>
@@ -5778,10 +5750,10 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5804,13 +5776,13 @@
         <v>89</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" s="2"/>
@@ -5861,7 +5833,7 @@
         <v>20</v>
       </c>
       <c r="AF30" t="s" s="2">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="AG30" t="s" s="2">
         <v>79</v>
@@ -5876,7 +5848,7 @@
         <v>100</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="AL30" t="s" s="2">
         <v>20</v>
@@ -5885,7 +5857,7 @@
         <v>20</v>
       </c>
       <c r="AN30" t="s" s="2">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="AO30" t="s" s="2">
         <v>20</v>
@@ -5893,10 +5865,10 @@
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
@@ -5919,17 +5891,17 @@
         <v>89</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="P31" t="s" s="2">
         <v>20</v>
@@ -5978,7 +5950,7 @@
         <v>20</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5993,7 +5965,7 @@
         <v>100</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="AL31" t="s" s="2">
         <v>20</v>
@@ -6002,7 +5974,7 @@
         <v>20</v>
       </c>
       <c r="AN31" t="s" s="2">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="AO31" t="s" s="2">
         <v>20</v>
@@ -6010,10 +5982,10 @@
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C32" t="s" s="2">
         <v>6</v>
@@ -6038,19 +6010,19 @@
         <v>89</v>
       </c>
       <c r="K32" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="L32" t="s" s="2">
+        <v>310</v>
+      </c>
+      <c r="M32" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="N32" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O32" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="L32" t="s" s="2">
-        <v>314</v>
-      </c>
-      <c r="M32" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N32" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="O32" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="P32" t="s" s="2">
         <v>20</v>
@@ -6060,7 +6032,7 @@
         <v>20</v>
       </c>
       <c r="S32" t="s" s="2">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="T32" t="s" s="2">
         <v>20</v>
@@ -6099,7 +6071,7 @@
         <v>20</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>79</v>
@@ -6114,16 +6086,16 @@
         <v>100</v>
       </c>
       <c r="AK32" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM32" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN32" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AO32" t="s" s="2">
         <v>20</v>
@@ -6131,13 +6103,13 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C33" t="s" s="2">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="D33" t="s" s="2">
         <v>20</v>
@@ -6159,19 +6131,19 @@
         <v>89</v>
       </c>
       <c r="K33" t="s" s="2">
+        <v>246</v>
+      </c>
+      <c r="L33" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="M33" t="s" s="2">
+        <v>248</v>
+      </c>
+      <c r="N33" t="s" s="2">
+        <v>249</v>
+      </c>
+      <c r="O33" t="s" s="2">
         <v>250</v>
-      </c>
-      <c r="L33" t="s" s="2">
-        <v>317</v>
-      </c>
-      <c r="M33" t="s" s="2">
-        <v>252</v>
-      </c>
-      <c r="N33" t="s" s="2">
-        <v>253</v>
-      </c>
-      <c r="O33" t="s" s="2">
-        <v>254</v>
       </c>
       <c r="P33" t="s" s="2">
         <v>20</v>
@@ -6181,7 +6153,7 @@
         <v>20</v>
       </c>
       <c r="S33" t="s" s="2">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="T33" t="s" s="2">
         <v>20</v>
@@ -6220,7 +6192,7 @@
         <v>20</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>79</v>
@@ -6235,16 +6207,16 @@
         <v>100</v>
       </c>
       <c r="AK33" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AL33" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="AM33" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN33" t="s" s="2">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="AO33" t="s" s="2">
         <v>20</v>
@@ -6252,10 +6224,10 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -6278,19 +6250,19 @@
         <v>89</v>
       </c>
       <c r="K34" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="L34" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="M34" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="N34" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="O34" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L34" t="s" s="2">
-        <v>321</v>
-      </c>
-      <c r="M34" t="s" s="2">
-        <v>322</v>
-      </c>
-      <c r="N34" t="s" s="2">
-        <v>323</v>
-      </c>
-      <c r="O34" t="s" s="2">
-        <v>324</v>
       </c>
       <c r="P34" t="s" s="2">
         <v>20</v>
@@ -6339,7 +6311,7 @@
         <v>20</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>79</v>
@@ -6354,16 +6326,16 @@
         <v>100</v>
       </c>
       <c r="AK34" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AL34" t="s" s="2">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="AM34" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="AO34" t="s" s="2">
         <v>20</v>
@@ -6371,10 +6343,10 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6400,16 +6372,16 @@
         <v>108</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="N35" t="s" s="2">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="O35" t="s" s="2">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="P35" t="s" s="2">
         <v>20</v>
@@ -6434,13 +6406,13 @@
         <v>20</v>
       </c>
       <c r="X35" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y35" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="Z35" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AA35" t="s" s="2">
         <v>20</v>
@@ -6458,7 +6430,7 @@
         <v>20</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -6473,16 +6445,16 @@
         <v>100</v>
       </c>
       <c r="AK35" t="s" s="2">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AL35" t="s" s="2">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="AM35" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN35" t="s" s="2">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="AO35" t="s" s="2">
         <v>20</v>
@@ -6490,10 +6462,10 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6516,19 +6488,19 @@
         <v>89</v>
       </c>
       <c r="K36" t="s" s="2">
+        <v>335</v>
+      </c>
+      <c r="L36" t="s" s="2">
+        <v>336</v>
+      </c>
+      <c r="M36" t="s" s="2">
+        <v>337</v>
+      </c>
+      <c r="N36" t="s" s="2">
+        <v>338</v>
+      </c>
+      <c r="O36" t="s" s="2">
         <v>339</v>
-      </c>
-      <c r="L36" t="s" s="2">
-        <v>340</v>
-      </c>
-      <c r="M36" t="s" s="2">
-        <v>341</v>
-      </c>
-      <c r="N36" t="s" s="2">
-        <v>342</v>
-      </c>
-      <c r="O36" t="s" s="2">
-        <v>343</v>
       </c>
       <c r="P36" t="s" s="2">
         <v>20</v>
@@ -6577,7 +6549,7 @@
         <v>20</v>
       </c>
       <c r="AF36" t="s" s="2">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="AG36" t="s" s="2">
         <v>79</v>
@@ -6592,27 +6564,27 @@
         <v>100</v>
       </c>
       <c r="AK36" t="s" s="2">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="AM36" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN36" t="s" s="2">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="AO36" t="s" s="2">
-        <v>347</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6635,19 +6607,19 @@
         <v>89</v>
       </c>
       <c r="K37" t="s" s="2">
+        <v>345</v>
+      </c>
+      <c r="L37" t="s" s="2">
+        <v>346</v>
+      </c>
+      <c r="M37" t="s" s="2">
+        <v>347</v>
+      </c>
+      <c r="N37" t="s" s="2">
+        <v>348</v>
+      </c>
+      <c r="O37" t="s" s="2">
         <v>349</v>
-      </c>
-      <c r="L37" t="s" s="2">
-        <v>350</v>
-      </c>
-      <c r="M37" t="s" s="2">
-        <v>351</v>
-      </c>
-      <c r="N37" t="s" s="2">
-        <v>352</v>
-      </c>
-      <c r="O37" t="s" s="2">
-        <v>353</v>
       </c>
       <c r="P37" t="s" s="2">
         <v>20</v>
@@ -6696,7 +6668,7 @@
         <v>20</v>
       </c>
       <c r="AF37" t="s" s="2">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="AG37" t="s" s="2">
         <v>79</v>
@@ -6711,16 +6683,16 @@
         <v>100</v>
       </c>
       <c r="AK37" t="s" s="2">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM37" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN37" t="s" s="2">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="AO37" t="s" s="2">
         <v>20</v>
@@ -6728,10 +6700,10 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
@@ -6751,22 +6723,22 @@
         <v>20</v>
       </c>
       <c r="J38" t="s" s="2">
-        <v>20</v>
+        <v>89</v>
       </c>
       <c r="K38" t="s" s="2">
+        <v>353</v>
+      </c>
+      <c r="L38" t="s" s="2">
+        <v>354</v>
+      </c>
+      <c r="M38" t="s" s="2">
+        <v>355</v>
+      </c>
+      <c r="N38" t="s" s="2">
+        <v>356</v>
+      </c>
+      <c r="O38" t="s" s="2">
         <v>357</v>
-      </c>
-      <c r="L38" t="s" s="2">
-        <v>358</v>
-      </c>
-      <c r="M38" t="s" s="2">
-        <v>359</v>
-      </c>
-      <c r="N38" t="s" s="2">
-        <v>360</v>
-      </c>
-      <c r="O38" t="s" s="2">
-        <v>361</v>
       </c>
       <c r="P38" t="s" s="2">
         <v>20</v>
@@ -6779,7 +6751,7 @@
         <v>20</v>
       </c>
       <c r="T38" t="s" s="2">
-        <v>362</v>
+        <v>20</v>
       </c>
       <c r="U38" t="s" s="2">
         <v>20</v>
@@ -6815,7 +6787,7 @@
         <v>20</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6824,22 +6796,22 @@
         <v>80</v>
       </c>
       <c r="AI38" t="s" s="2">
-        <v>162</v>
+        <v>20</v>
       </c>
       <c r="AJ38" t="s" s="2">
-        <v>363</v>
+        <v>100</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>20</v>
+        <v>359</v>
       </c>
       <c r="AM38" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN38" t="s" s="2">
-        <v>365</v>
+        <v>360</v>
       </c>
       <c r="AO38" t="s" s="2">
         <v>20</v>
@@ -6847,10 +6819,10 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>366</v>
+        <v>361</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6873,13 +6845,13 @@
         <v>20</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6930,7 +6902,7 @@
         <v>20</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>79</v>
@@ -6945,7 +6917,7 @@
         <v>20</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL39" t="s" s="2">
         <v>20</v>
@@ -6962,10 +6934,10 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6994,7 +6966,7 @@
         <v>135</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N40" t="s" s="2">
         <v>137</v>
@@ -7035,10 +7007,10 @@
         <v>20</v>
       </c>
       <c r="AB40" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AC40" t="s" s="2">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="AD40" t="s" s="2">
         <v>20</v>
@@ -7047,7 +7019,7 @@
         <v>151</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>79</v>
@@ -7062,7 +7034,7 @@
         <v>139</v>
       </c>
       <c r="AK40" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL40" t="s" s="2">
         <v>20</v>
@@ -7079,13 +7051,13 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>368</v>
+        <v>363</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>367</v>
+        <v>362</v>
       </c>
       <c r="C41" t="s" s="2">
-        <v>369</v>
+        <v>364</v>
       </c>
       <c r="D41" t="s" s="2">
         <v>20</v>
@@ -7107,13 +7079,13 @@
         <v>20</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>370</v>
+        <v>365</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>372</v>
+        <v>367</v>
       </c>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
@@ -7164,7 +7136,7 @@
         <v>20</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -7179,7 +7151,7 @@
         <v>139</v>
       </c>
       <c r="AK41" t="s" s="2">
-        <v>373</v>
+        <v>368</v>
       </c>
       <c r="AL41" t="s" s="2">
         <v>20</v>
@@ -7196,10 +7168,10 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>374</v>
+        <v>369</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -7225,16 +7197,16 @@
         <v>108</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>375</v>
+        <v>370</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>376</v>
+        <v>371</v>
       </c>
       <c r="N42" t="s" s="2">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="O42" t="s" s="2">
-        <v>378</v>
+        <v>373</v>
       </c>
       <c r="P42" t="s" s="2">
         <v>20</v>
@@ -7247,7 +7219,7 @@
         <v>20</v>
       </c>
       <c r="T42" t="s" s="2">
-        <v>379</v>
+        <v>374</v>
       </c>
       <c r="U42" t="s" s="2">
         <v>20</v>
@@ -7259,13 +7231,13 @@
         <v>20</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>380</v>
+        <v>375</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>20</v>
@@ -7283,7 +7255,7 @@
         <v>20</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>382</v>
+        <v>377</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -7298,7 +7270,7 @@
         <v>100</v>
       </c>
       <c r="AK42" t="s" s="2">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="AL42" t="s" s="2">
         <v>20</v>
@@ -7307,7 +7279,7 @@
         <v>20</v>
       </c>
       <c r="AN42" t="s" s="2">
-        <v>383</v>
+        <v>378</v>
       </c>
       <c r="AO42" t="s" s="2">
         <v>20</v>
@@ -7315,10 +7287,10 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>384</v>
+        <v>379</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7344,13 +7316,13 @@
         <v>108</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>385</v>
+        <v>380</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="N43" t="s" s="2">
-        <v>387</v>
+        <v>382</v>
       </c>
       <c r="O43" s="2"/>
       <c r="P43" t="s" s="2">
@@ -7364,7 +7336,7 @@
         <v>20</v>
       </c>
       <c r="T43" t="s" s="2">
-        <v>388</v>
+        <v>383</v>
       </c>
       <c r="U43" t="s" s="2">
         <v>20</v>
@@ -7376,13 +7348,13 @@
         <v>20</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>389</v>
+        <v>384</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>390</v>
+        <v>385</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>20</v>
@@ -7400,7 +7372,7 @@
         <v>20</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -7415,7 +7387,7 @@
         <v>100</v>
       </c>
       <c r="AK43" t="s" s="2">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="AL43" t="s" s="2">
         <v>20</v>
@@ -7424,7 +7396,7 @@
         <v>20</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>392</v>
+        <v>387</v>
       </c>
       <c r="AO43" t="s" s="2">
         <v>20</v>
@@ -7432,10 +7404,10 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>393</v>
+        <v>388</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
@@ -7458,19 +7430,19 @@
         <v>89</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>394</v>
+        <v>389</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>395</v>
+        <v>390</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>396</v>
+        <v>391</v>
       </c>
       <c r="O44" t="s" s="2">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="P44" t="s" s="2">
         <v>20</v>
@@ -7483,7 +7455,7 @@
         <v>20</v>
       </c>
       <c r="T44" t="s" s="2">
-        <v>397</v>
+        <v>392</v>
       </c>
       <c r="U44" t="s" s="2">
         <v>20</v>
@@ -7519,7 +7491,7 @@
         <v>20</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>398</v>
+        <v>393</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -7534,7 +7506,7 @@
         <v>100</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="AL44" t="s" s="2">
         <v>20</v>
@@ -7543,7 +7515,7 @@
         <v>20</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>399</v>
+        <v>394</v>
       </c>
       <c r="AO44" t="s" s="2">
         <v>20</v>
@@ -7551,10 +7523,10 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>400</v>
+        <v>395</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7565,7 +7537,7 @@
         <v>79</v>
       </c>
       <c r="G45" t="s" s="2">
-        <v>401</v>
+        <v>396</v>
       </c>
       <c r="H45" t="s" s="2">
         <v>89</v>
@@ -7577,13 +7549,13 @@
         <v>89</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>402</v>
+        <v>397</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>403</v>
+        <v>398</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7598,7 +7570,7 @@
         <v>20</v>
       </c>
       <c r="T45" t="s" s="2">
-        <v>404</v>
+        <v>399</v>
       </c>
       <c r="U45" t="s" s="2">
         <v>20</v>
@@ -7634,7 +7606,7 @@
         <v>20</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>405</v>
+        <v>400</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7649,7 +7621,7 @@
         <v>100</v>
       </c>
       <c r="AK45" t="s" s="2">
-        <v>406</v>
+        <v>401</v>
       </c>
       <c r="AL45" t="s" s="2">
         <v>20</v>
@@ -7658,7 +7630,7 @@
         <v>20</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="AO45" t="s" s="2">
         <v>20</v>
@@ -7666,10 +7638,10 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
@@ -7692,13 +7664,13 @@
         <v>20</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7749,7 +7721,7 @@
         <v>20</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7781,10 +7753,10 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7810,10 +7782,10 @@
         <v>134</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7852,7 +7824,7 @@
         <v>20</v>
       </c>
       <c r="AB47" t="s" s="2">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="AC47" s="2"/>
       <c r="AD47" t="s" s="2">
@@ -7862,7 +7834,7 @@
         <v>151</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7894,13 +7866,13 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C48" t="s" s="2">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="D48" t="s" s="2">
         <v>20</v>
@@ -7922,13 +7894,13 @@
         <v>20</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>417</v>
+        <v>412</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>418</v>
+        <v>413</v>
       </c>
       <c r="N48" s="2"/>
       <c r="O48" s="2"/>
@@ -7979,7 +7951,7 @@
         <v>20</v>
       </c>
       <c r="AF48" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG48" t="s" s="2">
         <v>79</v>
@@ -7994,7 +7966,7 @@
         <v>139</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>419</v>
+        <v>414</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>20</v>
@@ -8011,13 +7983,13 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>420</v>
+        <v>415</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C49" t="s" s="2">
-        <v>421</v>
+        <v>416</v>
       </c>
       <c r="D49" t="s" s="2">
         <v>20</v>
@@ -8039,13 +8011,13 @@
         <v>20</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>423</v>
+        <v>418</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="N49" s="2"/>
       <c r="O49" s="2"/>
@@ -8096,7 +8068,7 @@
         <v>20</v>
       </c>
       <c r="AF49" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG49" t="s" s="2">
         <v>79</v>
@@ -8111,7 +8083,7 @@
         <v>139</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>425</v>
+        <v>420</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>20</v>
@@ -8128,13 +8100,13 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C50" t="s" s="2">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D50" t="s" s="2">
         <v>20</v>
@@ -8156,13 +8128,13 @@
         <v>20</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>428</v>
+        <v>423</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>429</v>
+        <v>424</v>
       </c>
       <c r="N50" s="2"/>
       <c r="O50" s="2"/>
@@ -8213,7 +8185,7 @@
         <v>20</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -8228,7 +8200,7 @@
         <v>139</v>
       </c>
       <c r="AK50" t="s" s="2">
-        <v>430</v>
+        <v>425</v>
       </c>
       <c r="AL50" t="s" s="2">
         <v>20</v>
@@ -8245,13 +8217,13 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>431</v>
+        <v>426</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="C51" t="s" s="2">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="D51" t="s" s="2">
         <v>20</v>
@@ -8273,13 +8245,13 @@
         <v>20</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>433</v>
+        <v>428</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>432</v>
+        <v>427</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>434</v>
+        <v>429</v>
       </c>
       <c r="N51" s="2"/>
       <c r="O51" s="2"/>
@@ -8330,7 +8302,7 @@
         <v>20</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -8345,7 +8317,7 @@
         <v>139</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>435</v>
+        <v>430</v>
       </c>
       <c r="AL51" t="s" s="2">
         <v>20</v>
@@ -8362,10 +8334,10 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>436</v>
+        <v>431</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8388,13 +8360,13 @@
         <v>20</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>437</v>
+        <v>432</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>438</v>
+        <v>433</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -8418,7 +8390,7 @@
         <v>20</v>
       </c>
       <c r="W52" t="s" s="2">
-        <v>439</v>
+        <v>434</v>
       </c>
       <c r="X52" t="s" s="2">
         <v>20</v>
@@ -8445,7 +8417,7 @@
         <v>20</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -8477,14 +8449,14 @@
     </row>
     <row r="53" hidden="true">
       <c r="A53" t="s" s="2">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="E53" s="2"/>
       <c r="F53" t="s" s="2">
@@ -8503,13 +8475,13 @@
         <v>89</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>443</v>
+        <v>438</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>444</v>
+        <v>439</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -8524,7 +8496,7 @@
         <v>20</v>
       </c>
       <c r="T53" t="s" s="2">
-        <v>445</v>
+        <v>440</v>
       </c>
       <c r="U53" t="s" s="2">
         <v>20</v>
@@ -8560,7 +8532,7 @@
         <v>20</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>446</v>
+        <v>441</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>79</v>
@@ -8575,7 +8547,7 @@
         <v>100</v>
       </c>
       <c r="AK53" t="s" s="2">
-        <v>447</v>
+        <v>442</v>
       </c>
       <c r="AL53" t="s" s="2">
         <v>20</v>
@@ -8584,7 +8556,7 @@
         <v>20</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>448</v>
+        <v>443</v>
       </c>
       <c r="AO53" t="s" s="2">
         <v>20</v>
@@ -8592,14 +8564,14 @@
     </row>
     <row r="54" hidden="true">
       <c r="A54" t="s" s="2">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>449</v>
+        <v>444</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
-        <v>450</v>
+        <v>445</v>
       </c>
       <c r="E54" s="2"/>
       <c r="F54" t="s" s="2">
@@ -8618,16 +8590,16 @@
         <v>89</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>451</v>
+        <v>446</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>452</v>
+        <v>447</v>
       </c>
       <c r="N54" t="s" s="2">
-        <v>453</v>
+        <v>448</v>
       </c>
       <c r="O54" s="2"/>
       <c r="P54" t="s" s="2">
@@ -8641,7 +8613,7 @@
         <v>20</v>
       </c>
       <c r="T54" t="s" s="2">
-        <v>454</v>
+        <v>449</v>
       </c>
       <c r="U54" t="s" s="2">
         <v>20</v>
@@ -8677,7 +8649,7 @@
         <v>20</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>455</v>
+        <v>450</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>79</v>
@@ -8692,7 +8664,7 @@
         <v>100</v>
       </c>
       <c r="AK54" t="s" s="2">
-        <v>456</v>
+        <v>451</v>
       </c>
       <c r="AL54" t="s" s="2">
         <v>20</v>
@@ -8701,7 +8673,7 @@
         <v>20</v>
       </c>
       <c r="AN54" t="s" s="2">
-        <v>457</v>
+        <v>452</v>
       </c>
       <c r="AO54" t="s" s="2">
         <v>20</v>
@@ -8709,14 +8681,14 @@
     </row>
     <row r="55" hidden="true">
       <c r="A55" t="s" s="2">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>458</v>
+        <v>453</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
-        <v>459</v>
+        <v>454</v>
       </c>
       <c r="E55" s="2"/>
       <c r="F55" t="s" s="2">
@@ -8735,13 +8707,13 @@
         <v>89</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>460</v>
+        <v>455</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>461</v>
+        <v>456</v>
       </c>
       <c r="N55" s="2"/>
       <c r="O55" s="2"/>
@@ -8772,7 +8744,7 @@
       </c>
       <c r="Y55" s="2"/>
       <c r="Z55" t="s" s="2">
-        <v>462</v>
+        <v>457</v>
       </c>
       <c r="AA55" t="s" s="2">
         <v>20</v>
@@ -8790,7 +8762,7 @@
         <v>20</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>463</v>
+        <v>458</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>79</v>
@@ -8805,7 +8777,7 @@
         <v>100</v>
       </c>
       <c r="AK55" t="s" s="2">
-        <v>464</v>
+        <v>459</v>
       </c>
       <c r="AL55" t="s" s="2">
         <v>20</v>
@@ -8814,7 +8786,7 @@
         <v>20</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>465</v>
+        <v>460</v>
       </c>
       <c r="AO55" t="s" s="2">
         <v>20</v>
@@ -8822,14 +8794,14 @@
     </row>
     <row r="56" hidden="true">
       <c r="A56" t="s" s="2">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>466</v>
+        <v>461</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
-        <v>467</v>
+        <v>462</v>
       </c>
       <c r="E56" s="2"/>
       <c r="F56" t="s" s="2">
@@ -8848,13 +8820,13 @@
         <v>89</v>
       </c>
       <c r="K56" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L56" t="s" s="2">
-        <v>468</v>
+        <v>463</v>
       </c>
       <c r="M56" t="s" s="2">
-        <v>469</v>
+        <v>464</v>
       </c>
       <c r="N56" s="2"/>
       <c r="O56" s="2"/>
@@ -8869,7 +8841,7 @@
         <v>20</v>
       </c>
       <c r="T56" t="s" s="2">
-        <v>470</v>
+        <v>465</v>
       </c>
       <c r="U56" t="s" s="2">
         <v>20</v>
@@ -8905,7 +8877,7 @@
         <v>20</v>
       </c>
       <c r="AF56" t="s" s="2">
-        <v>471</v>
+        <v>466</v>
       </c>
       <c r="AG56" t="s" s="2">
         <v>79</v>
@@ -8920,7 +8892,7 @@
         <v>100</v>
       </c>
       <c r="AK56" t="s" s="2">
-        <v>472</v>
+        <v>467</v>
       </c>
       <c r="AL56" t="s" s="2">
         <v>20</v>
@@ -8929,7 +8901,7 @@
         <v>20</v>
       </c>
       <c r="AN56" t="s" s="2">
-        <v>473</v>
+        <v>468</v>
       </c>
       <c r="AO56" t="s" s="2">
         <v>20</v>
@@ -8937,10 +8909,10 @@
     </row>
     <row r="57" hidden="true">
       <c r="A57" t="s" s="2">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>474</v>
+        <v>469</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8963,16 +8935,16 @@
         <v>89</v>
       </c>
       <c r="K57" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L57" t="s" s="2">
-        <v>475</v>
+        <v>470</v>
       </c>
       <c r="M57" t="s" s="2">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="N57" t="s" s="2">
-        <v>477</v>
+        <v>472</v>
       </c>
       <c r="O57" s="2"/>
       <c r="P57" t="s" s="2">
@@ -8998,11 +8970,11 @@
         <v>20</v>
       </c>
       <c r="X57" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y57" s="2"/>
       <c r="Z57" t="s" s="2">
-        <v>478</v>
+        <v>473</v>
       </c>
       <c r="AA57" t="s" s="2">
         <v>20</v>
@@ -9020,7 +8992,7 @@
         <v>20</v>
       </c>
       <c r="AF57" t="s" s="2">
-        <v>479</v>
+        <v>474</v>
       </c>
       <c r="AG57" t="s" s="2">
         <v>79</v>
@@ -9035,7 +9007,7 @@
         <v>100</v>
       </c>
       <c r="AK57" t="s" s="2">
-        <v>480</v>
+        <v>475</v>
       </c>
       <c r="AL57" t="s" s="2">
         <v>20</v>
@@ -9044,7 +9016,7 @@
         <v>20</v>
       </c>
       <c r="AN57" t="s" s="2">
-        <v>481</v>
+        <v>476</v>
       </c>
       <c r="AO57" t="s" s="2">
         <v>20</v>
@@ -9052,10 +9024,10 @@
     </row>
     <row r="58" hidden="true">
       <c r="A58" t="s" s="2">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>482</v>
+        <v>477</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -9078,17 +9050,17 @@
         <v>89</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>483</v>
+        <v>478</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>484</v>
+        <v>479</v>
       </c>
       <c r="N58" s="2"/>
       <c r="O58" t="s" s="2">
-        <v>485</v>
+        <v>480</v>
       </c>
       <c r="P58" t="s" s="2">
         <v>20</v>
@@ -9101,7 +9073,7 @@
         <v>20</v>
       </c>
       <c r="T58" t="s" s="2">
-        <v>486</v>
+        <v>481</v>
       </c>
       <c r="U58" t="s" s="2">
         <v>20</v>
@@ -9137,7 +9109,7 @@
         <v>20</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>487</v>
+        <v>482</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>79</v>
@@ -9152,7 +9124,7 @@
         <v>100</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>20</v>
@@ -9161,7 +9133,7 @@
         <v>20</v>
       </c>
       <c r="AN58" t="s" s="2">
-        <v>488</v>
+        <v>483</v>
       </c>
       <c r="AO58" t="s" s="2">
         <v>20</v>
@@ -9169,10 +9141,10 @@
     </row>
     <row r="59" hidden="true">
       <c r="A59" t="s" s="2">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9195,17 +9167,17 @@
         <v>20</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>490</v>
+        <v>485</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>491</v>
+        <v>486</v>
       </c>
       <c r="N59" s="2"/>
       <c r="O59" t="s" s="2">
-        <v>492</v>
+        <v>487</v>
       </c>
       <c r="P59" t="s" s="2">
         <v>20</v>
@@ -9230,13 +9202,13 @@
         <v>20</v>
       </c>
       <c r="X59" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Y59" t="s" s="2">
-        <v>493</v>
+        <v>488</v>
       </c>
       <c r="Z59" t="s" s="2">
-        <v>494</v>
+        <v>489</v>
       </c>
       <c r="AA59" t="s" s="2">
         <v>20</v>
@@ -9254,7 +9226,7 @@
         <v>20</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>489</v>
+        <v>484</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -9269,16 +9241,16 @@
         <v>100</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>495</v>
+        <v>490</v>
       </c>
       <c r="AL59" t="s" s="2">
-        <v>496</v>
+        <v>491</v>
       </c>
       <c r="AM59" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN59" t="s" s="2">
-        <v>497</v>
+        <v>492</v>
       </c>
       <c r="AO59" t="s" s="2">
         <v>20</v>
@@ -9286,10 +9258,10 @@
     </row>
     <row r="60" hidden="true">
       <c r="A60" t="s" s="2">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9312,19 +9284,19 @@
         <v>20</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>499</v>
+        <v>494</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>500</v>
+        <v>495</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>502</v>
+        <v>497</v>
       </c>
       <c r="O60" t="s" s="2">
-        <v>503</v>
+        <v>498</v>
       </c>
       <c r="P60" t="s" s="2">
         <v>20</v>
@@ -9373,7 +9345,7 @@
         <v>20</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>498</v>
+        <v>493</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>79</v>
@@ -9388,16 +9360,16 @@
         <v>100</v>
       </c>
       <c r="AK60" t="s" s="2">
-        <v>504</v>
+        <v>499</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM60" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN60" t="s" s="2">
-        <v>505</v>
+        <v>500</v>
       </c>
       <c r="AO60" t="s" s="2">
         <v>20</v>
@@ -9405,10 +9377,10 @@
     </row>
     <row r="61" hidden="true">
       <c r="A61" t="s" s="2">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
@@ -9431,19 +9403,19 @@
         <v>20</v>
       </c>
       <c r="K61" t="s" s="2">
-        <v>507</v>
+        <v>502</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>508</v>
+        <v>503</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>509</v>
+        <v>504</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>510</v>
+        <v>505</v>
       </c>
       <c r="O61" t="s" s="2">
-        <v>511</v>
+        <v>506</v>
       </c>
       <c r="P61" t="s" s="2">
         <v>20</v>
@@ -9492,7 +9464,7 @@
         <v>20</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>506</v>
+        <v>501</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -9507,16 +9479,16 @@
         <v>100</v>
       </c>
       <c r="AK61" t="s" s="2">
-        <v>512</v>
+        <v>507</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM61" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>513</v>
+        <v>508</v>
       </c>
       <c r="AO61" t="s" s="2">
         <v>20</v>
@@ -9524,10 +9496,10 @@
     </row>
     <row r="62" hidden="true">
       <c r="A62" t="s" s="2">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
@@ -9550,19 +9522,19 @@
         <v>20</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>516</v>
+        <v>511</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>517</v>
+        <v>512</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>518</v>
+        <v>513</v>
       </c>
       <c r="O62" t="s" s="2">
-        <v>519</v>
+        <v>514</v>
       </c>
       <c r="P62" t="s" s="2">
         <v>20</v>
@@ -9611,7 +9583,7 @@
         <v>20</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9623,13 +9595,13 @@
         <v>20</v>
       </c>
       <c r="AJ62" t="s" s="2">
-        <v>520</v>
+        <v>515</v>
       </c>
       <c r="AK62" t="s" s="2">
-        <v>521</v>
+        <v>516</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM62" t="s" s="2">
         <v>20</v>
@@ -9643,10 +9615,10 @@
     </row>
     <row r="63" hidden="true">
       <c r="A63" t="s" s="2">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>522</v>
+        <v>517</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9669,13 +9641,13 @@
         <v>20</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9726,7 +9698,7 @@
         <v>20</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>79</v>
@@ -9741,7 +9713,7 @@
         <v>20</v>
       </c>
       <c r="AK63" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL63" t="s" s="2">
         <v>20</v>
@@ -9758,10 +9730,10 @@
     </row>
     <row r="64" hidden="true">
       <c r="A64" t="s" s="2">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>523</v>
+        <v>518</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9790,7 +9762,7 @@
         <v>135</v>
       </c>
       <c r="M64" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N64" t="s" s="2">
         <v>137</v>
@@ -9843,7 +9815,7 @@
         <v>20</v>
       </c>
       <c r="AF64" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG64" t="s" s="2">
         <v>79</v>
@@ -9858,7 +9830,7 @@
         <v>139</v>
       </c>
       <c r="AK64" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL64" t="s" s="2">
         <v>20</v>
@@ -9875,14 +9847,14 @@
     </row>
     <row r="65" hidden="true">
       <c r="A65" t="s" s="2">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>524</v>
+        <v>519</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" t="s" s="2">
@@ -9904,10 +9876,10 @@
         <v>134</v>
       </c>
       <c r="L65" t="s" s="2">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="M65" t="s" s="2">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="N65" t="s" s="2">
         <v>137</v>
@@ -9962,7 +9934,7 @@
         <v>20</v>
       </c>
       <c r="AF65" t="s" s="2">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="AG65" t="s" s="2">
         <v>79</v>
@@ -9994,10 +9966,10 @@
     </row>
     <row r="66" hidden="true">
       <c r="A66" t="s" s="2">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
@@ -10020,17 +9992,17 @@
         <v>20</v>
       </c>
       <c r="K66" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>530</v>
+        <v>525</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>531</v>
+        <v>526</v>
       </c>
       <c r="N66" s="2"/>
       <c r="O66" t="s" s="2">
-        <v>532</v>
+        <v>527</v>
       </c>
       <c r="P66" t="s" s="2">
         <v>20</v>
@@ -10055,13 +10027,13 @@
         <v>20</v>
       </c>
       <c r="X66" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="Y66" t="s" s="2">
-        <v>533</v>
+        <v>528</v>
       </c>
       <c r="Z66" t="s" s="2">
-        <v>534</v>
+        <v>529</v>
       </c>
       <c r="AA66" t="s" s="2">
         <v>20</v>
@@ -10079,7 +10051,7 @@
         <v>20</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>529</v>
+        <v>524</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>79</v>
@@ -10094,16 +10066,16 @@
         <v>100</v>
       </c>
       <c r="AK66" t="s" s="2">
-        <v>535</v>
+        <v>530</v>
       </c>
       <c r="AL66" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM66" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN66" t="s" s="2">
-        <v>536</v>
+        <v>531</v>
       </c>
       <c r="AO66" t="s" s="2">
         <v>20</v>
@@ -10111,10 +10083,10 @@
     </row>
     <row r="67" hidden="true">
       <c r="A67" t="s" s="2">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
@@ -10137,17 +10109,17 @@
         <v>20</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>538</v>
+        <v>533</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>539</v>
+        <v>534</v>
       </c>
       <c r="N67" s="2"/>
       <c r="O67" t="s" s="2">
-        <v>540</v>
+        <v>535</v>
       </c>
       <c r="P67" t="s" s="2">
         <v>20</v>
@@ -10196,7 +10168,7 @@
         <v>20</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>537</v>
+        <v>532</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>79</v>
@@ -10211,16 +10183,16 @@
         <v>100</v>
       </c>
       <c r="AK67" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM67" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>541</v>
+        <v>536</v>
       </c>
       <c r="AO67" t="s" s="2">
         <v>20</v>
@@ -10228,10 +10200,10 @@
     </row>
     <row r="68" hidden="true">
       <c r="A68" t="s" s="2">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10254,19 +10226,19 @@
         <v>20</v>
       </c>
       <c r="K68" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="L68" t="s" s="2">
+        <v>538</v>
+      </c>
+      <c r="M68" t="s" s="2">
+        <v>539</v>
+      </c>
+      <c r="N68" t="s" s="2">
+        <v>540</v>
+      </c>
+      <c r="O68" t="s" s="2">
         <v>320</v>
-      </c>
-      <c r="L68" t="s" s="2">
-        <v>543</v>
-      </c>
-      <c r="M68" t="s" s="2">
-        <v>544</v>
-      </c>
-      <c r="N68" t="s" s="2">
-        <v>545</v>
-      </c>
-      <c r="O68" t="s" s="2">
-        <v>324</v>
       </c>
       <c r="P68" t="s" s="2">
         <v>20</v>
@@ -10315,7 +10287,7 @@
         <v>20</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>542</v>
+        <v>537</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -10330,16 +10302,16 @@
         <v>100</v>
       </c>
       <c r="AK68" t="s" s="2">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="AL68" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM68" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN68" t="s" s="2">
-        <v>546</v>
+        <v>541</v>
       </c>
       <c r="AO68" t="s" s="2">
         <v>20</v>
@@ -10347,10 +10319,10 @@
     </row>
     <row r="69" hidden="true">
       <c r="A69" t="s" s="2">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10373,17 +10345,17 @@
         <v>20</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>548</v>
+        <v>543</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>549</v>
+        <v>544</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>550</v>
+        <v>545</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" t="s" s="2">
-        <v>551</v>
+        <v>546</v>
       </c>
       <c r="P69" t="s" s="2">
         <v>20</v>
@@ -10432,7 +10404,7 @@
         <v>20</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>547</v>
+        <v>542</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -10447,16 +10419,16 @@
         <v>100</v>
       </c>
       <c r="AK69" t="s" s="2">
-        <v>552</v>
+        <v>358</v>
       </c>
       <c r="AL69" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM69" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN69" t="s" s="2">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="AO69" t="s" s="2">
         <v>20</v>
@@ -10464,10 +10436,10 @@
     </row>
     <row r="70" hidden="true">
       <c r="A70" t="s" s="2">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10493,14 +10465,14 @@
         <v>108</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="N70" s="2"/>
       <c r="O70" t="s" s="2">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="P70" t="s" s="2">
         <v>20</v>
@@ -10525,13 +10497,13 @@
         <v>20</v>
       </c>
       <c r="X70" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y70" t="s" s="2">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="Z70" t="s" s="2">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="AA70" t="s" s="2">
         <v>20</v>
@@ -10549,7 +10521,7 @@
         <v>20</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>79</v>
@@ -10564,16 +10536,16 @@
         <v>100</v>
       </c>
       <c r="AK70" t="s" s="2">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="AL70" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM70" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN70" t="s" s="2">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="AO70" t="s" s="2">
         <v>20</v>
@@ -10581,10 +10553,10 @@
     </row>
     <row r="71" hidden="true">
       <c r="A71" t="s" s="2">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10607,17 +10579,17 @@
         <v>20</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>560</v>
+        <v>554</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>561</v>
+        <v>555</v>
       </c>
       <c r="N71" s="2"/>
       <c r="O71" t="s" s="2">
-        <v>562</v>
+        <v>556</v>
       </c>
       <c r="P71" t="s" s="2">
         <v>20</v>
@@ -10666,7 +10638,7 @@
         <v>20</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>79</v>
@@ -10675,22 +10647,22 @@
         <v>88</v>
       </c>
       <c r="AI71" t="s" s="2">
-        <v>563</v>
+        <v>557</v>
       </c>
       <c r="AJ71" t="s" s="2">
         <v>100</v>
       </c>
       <c r="AK71" t="s" s="2">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="AL71" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM71" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN71" t="s" s="2">
-        <v>565</v>
+        <v>559</v>
       </c>
       <c r="AO71" t="s" s="2">
         <v>20</v>
@@ -10698,10 +10670,10 @@
     </row>
     <row r="72" hidden="true">
       <c r="A72" t="s" s="2">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10724,13 +10696,13 @@
         <v>20</v>
       </c>
       <c r="K72" t="s" s="2">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="L72" t="s" s="2">
-        <v>567</v>
+        <v>561</v>
       </c>
       <c r="M72" t="s" s="2">
-        <v>568</v>
+        <v>562</v>
       </c>
       <c r="N72" s="2"/>
       <c r="O72" s="2"/>
@@ -10781,7 +10753,7 @@
         <v>20</v>
       </c>
       <c r="AF72" t="s" s="2">
-        <v>566</v>
+        <v>560</v>
       </c>
       <c r="AG72" t="s" s="2">
         <v>79</v>
@@ -10796,10 +10768,10 @@
         <v>100</v>
       </c>
       <c r="AK72" t="s" s="2">
-        <v>569</v>
+        <v>563</v>
       </c>
       <c r="AL72" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM72" t="s" s="2">
         <v>20</v>
@@ -10813,10 +10785,10 @@
     </row>
     <row r="73" hidden="true">
       <c r="A73" t="s" s="2">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10839,19 +10811,19 @@
         <v>20</v>
       </c>
       <c r="K73" t="s" s="2">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L73" t="s" s="2">
-        <v>571</v>
+        <v>565</v>
       </c>
       <c r="M73" t="s" s="2">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="N73" t="s" s="2">
-        <v>573</v>
+        <v>567</v>
       </c>
       <c r="O73" t="s" s="2">
-        <v>574</v>
+        <v>568</v>
       </c>
       <c r="P73" t="s" s="2">
         <v>20</v>
@@ -10900,7 +10872,7 @@
         <v>20</v>
       </c>
       <c r="AF73" t="s" s="2">
-        <v>570</v>
+        <v>564</v>
       </c>
       <c r="AG73" t="s" s="2">
         <v>79</v>
@@ -10915,10 +10887,10 @@
         <v>100</v>
       </c>
       <c r="AK73" t="s" s="2">
-        <v>575</v>
+        <v>569</v>
       </c>
       <c r="AL73" t="s" s="2">
-        <v>576</v>
+        <v>570</v>
       </c>
       <c r="AM73" t="s" s="2">
         <v>20</v>
@@ -10932,10 +10904,10 @@
     </row>
     <row r="74" hidden="true">
       <c r="A74" t="s" s="2">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>577</v>
+        <v>571</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
@@ -10958,13 +10930,13 @@
         <v>20</v>
       </c>
       <c r="K74" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N74" s="2"/>
       <c r="O74" s="2"/>
@@ -11015,7 +10987,7 @@
         <v>20</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
@@ -11030,7 +11002,7 @@
         <v>20</v>
       </c>
       <c r="AK74" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL74" t="s" s="2">
         <v>20</v>
@@ -11047,10 +11019,10 @@
     </row>
     <row r="75" hidden="true">
       <c r="A75" t="s" s="2">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>578</v>
+        <v>572</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -11079,7 +11051,7 @@
         <v>135</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N75" t="s" s="2">
         <v>137</v>
@@ -11132,7 +11104,7 @@
         <v>20</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -11147,7 +11119,7 @@
         <v>139</v>
       </c>
       <c r="AK75" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL75" t="s" s="2">
         <v>20</v>
@@ -11164,14 +11136,14 @@
     </row>
     <row r="76" hidden="true">
       <c r="A76" t="s" s="2">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>579</v>
+        <v>573</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E76" s="2"/>
       <c r="F76" t="s" s="2">
@@ -11193,10 +11165,10 @@
         <v>134</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="N76" t="s" s="2">
         <v>137</v>
@@ -11251,7 +11223,7 @@
         <v>20</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
@@ -11283,10 +11255,10 @@
     </row>
     <row r="77" hidden="true">
       <c r="A77" t="s" s="2">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11309,19 +11281,19 @@
         <v>20</v>
       </c>
       <c r="K77" t="s" s="2">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>581</v>
+        <v>575</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>582</v>
+        <v>576</v>
       </c>
       <c r="N77" t="s" s="2">
-        <v>583</v>
+        <v>577</v>
       </c>
       <c r="O77" t="s" s="2">
-        <v>584</v>
+        <v>578</v>
       </c>
       <c r="P77" t="s" s="2">
         <v>20</v>
@@ -11370,7 +11342,7 @@
         <v>20</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>580</v>
+        <v>574</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>88</v>
@@ -11385,16 +11357,16 @@
         <v>100</v>
       </c>
       <c r="AK77" t="s" s="2">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="AL77" t="s" s="2">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="AM77" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN77" t="s" s="2">
-        <v>587</v>
+        <v>581</v>
       </c>
       <c r="AO77" t="s" s="2">
         <v>20</v>
@@ -11402,10 +11374,10 @@
     </row>
     <row r="78" hidden="true">
       <c r="A78" t="s" s="2">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11428,19 +11400,19 @@
         <v>20</v>
       </c>
       <c r="K78" t="s" s="2">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>589</v>
+        <v>583</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>590</v>
+        <v>584</v>
       </c>
       <c r="N78" t="s" s="2">
-        <v>591</v>
+        <v>585</v>
       </c>
       <c r="O78" t="s" s="2">
-        <v>592</v>
+        <v>586</v>
       </c>
       <c r="P78" t="s" s="2">
         <v>20</v>
@@ -11489,7 +11461,7 @@
         <v>20</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>588</v>
+        <v>582</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>79</v>
@@ -11504,16 +11476,16 @@
         <v>100</v>
       </c>
       <c r="AK78" t="s" s="2">
-        <v>593</v>
+        <v>587</v>
       </c>
       <c r="AL78" t="s" s="2">
-        <v>594</v>
+        <v>588</v>
       </c>
       <c r="AM78" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN78" t="s" s="2">
-        <v>595</v>
+        <v>589</v>
       </c>
       <c r="AO78" t="s" s="2">
         <v>20</v>
@@ -11521,14 +11493,14 @@
     </row>
     <row r="79" hidden="true">
       <c r="A79" t="s" s="2">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
-        <v>597</v>
+        <v>591</v>
       </c>
       <c r="E79" s="2"/>
       <c r="F79" t="s" s="2">
@@ -11547,16 +11519,16 @@
         <v>20</v>
       </c>
       <c r="K79" t="s" s="2">
-        <v>598</v>
+        <v>592</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>599</v>
+        <v>593</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>600</v>
+        <v>594</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>601</v>
+        <v>595</v>
       </c>
       <c r="O79" s="2"/>
       <c r="P79" t="s" s="2">
@@ -11606,7 +11578,7 @@
         <v>20</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>596</v>
+        <v>590</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>79</v>
@@ -11621,16 +11593,16 @@
         <v>100</v>
       </c>
       <c r="AK79" t="s" s="2">
-        <v>602</v>
+        <v>596</v>
       </c>
       <c r="AL79" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM79" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN79" t="s" s="2">
-        <v>603</v>
+        <v>597</v>
       </c>
       <c r="AO79" t="s" s="2">
         <v>20</v>
@@ -11638,10 +11610,10 @@
     </row>
     <row r="80" hidden="true">
       <c r="A80" t="s" s="2">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11664,19 +11636,19 @@
         <v>89</v>
       </c>
       <c r="K80" t="s" s="2">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>605</v>
+        <v>599</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>606</v>
+        <v>600</v>
       </c>
       <c r="N80" t="s" s="2">
-        <v>607</v>
+        <v>601</v>
       </c>
       <c r="O80" t="s" s="2">
-        <v>608</v>
+        <v>602</v>
       </c>
       <c r="P80" t="s" s="2">
         <v>20</v>
@@ -11725,7 +11697,7 @@
         <v>20</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>604</v>
+        <v>598</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>79</v>
@@ -11740,10 +11712,10 @@
         <v>100</v>
       </c>
       <c r="AK80" t="s" s="2">
-        <v>564</v>
+        <v>558</v>
       </c>
       <c r="AL80" t="s" s="2">
-        <v>609</v>
+        <v>603</v>
       </c>
       <c r="AM80" t="s" s="2">
         <v>20</v>
@@ -11757,10 +11729,10 @@
     </row>
     <row r="81" hidden="true">
       <c r="A81" t="s" s="2">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11783,19 +11755,19 @@
         <v>89</v>
       </c>
       <c r="K81" t="s" s="2">
-        <v>515</v>
+        <v>510</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>611</v>
+        <v>605</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>612</v>
+        <v>606</v>
       </c>
       <c r="N81" t="s" s="2">
-        <v>613</v>
+        <v>607</v>
       </c>
       <c r="O81" t="s" s="2">
-        <v>614</v>
+        <v>608</v>
       </c>
       <c r="P81" t="s" s="2">
         <v>20</v>
@@ -11844,7 +11816,7 @@
         <v>20</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>610</v>
+        <v>604</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>79</v>
@@ -11859,10 +11831,10 @@
         <v>100</v>
       </c>
       <c r="AK81" t="s" s="2">
-        <v>615</v>
+        <v>609</v>
       </c>
       <c r="AL81" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM81" t="s" s="2">
         <v>20</v>
@@ -11876,10 +11848,10 @@
     </row>
     <row r="82" hidden="true">
       <c r="A82" t="s" s="2">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>616</v>
+        <v>610</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11902,13 +11874,13 @@
         <v>20</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -11959,7 +11931,7 @@
         <v>20</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>79</v>
@@ -11974,7 +11946,7 @@
         <v>20</v>
       </c>
       <c r="AK82" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL82" t="s" s="2">
         <v>20</v>
@@ -11991,10 +11963,10 @@
     </row>
     <row r="83" hidden="true">
       <c r="A83" t="s" s="2">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>617</v>
+        <v>611</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -12023,7 +11995,7 @@
         <v>135</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="N83" t="s" s="2">
         <v>137</v>
@@ -12076,7 +12048,7 @@
         <v>20</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
@@ -12091,7 +12063,7 @@
         <v>139</v>
       </c>
       <c r="AK83" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AL83" t="s" s="2">
         <v>20</v>
@@ -12108,14 +12080,14 @@
     </row>
     <row r="84" hidden="true">
       <c r="A84" t="s" s="2">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>618</v>
+        <v>612</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
-        <v>525</v>
+        <v>520</v>
       </c>
       <c r="E84" s="2"/>
       <c r="F84" t="s" s="2">
@@ -12137,10 +12109,10 @@
         <v>134</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>526</v>
+        <v>521</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>527</v>
+        <v>522</v>
       </c>
       <c r="N84" t="s" s="2">
         <v>137</v>
@@ -12195,7 +12167,7 @@
         <v>20</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>528</v>
+        <v>523</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>79</v>
@@ -12227,10 +12199,10 @@
     </row>
     <row r="85" hidden="true">
       <c r="A85" t="s" s="2">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12253,16 +12225,16 @@
         <v>89</v>
       </c>
       <c r="K85" t="s" s="2">
-        <v>620</v>
+        <v>614</v>
       </c>
       <c r="L85" t="s" s="2">
-        <v>621</v>
+        <v>615</v>
       </c>
       <c r="M85" t="s" s="2">
-        <v>622</v>
+        <v>616</v>
       </c>
       <c r="N85" t="s" s="2">
-        <v>623</v>
+        <v>617</v>
       </c>
       <c r="O85" s="2"/>
       <c r="P85" t="s" s="2">
@@ -12312,7 +12284,7 @@
         <v>20</v>
       </c>
       <c r="AF85" t="s" s="2">
-        <v>619</v>
+        <v>613</v>
       </c>
       <c r="AG85" t="s" s="2">
         <v>88</v>
@@ -12330,13 +12302,13 @@
         <v>152</v>
       </c>
       <c r="AL85" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM85" t="s" s="2">
         <v>20</v>
       </c>
       <c r="AN85" t="s" s="2">
-        <v>624</v>
+        <v>618</v>
       </c>
       <c r="AO85" t="s" s="2">
         <v>20</v>
@@ -12344,10 +12316,10 @@
     </row>
     <row r="86" hidden="true">
       <c r="A86" t="s" s="2">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12373,10 +12345,10 @@
         <v>108</v>
       </c>
       <c r="L86" t="s" s="2">
-        <v>626</v>
+        <v>620</v>
       </c>
       <c r="M86" t="s" s="2">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="N86" s="2"/>
       <c r="O86" s="2"/>
@@ -12403,13 +12375,13 @@
         <v>20</v>
       </c>
       <c r="X86" t="s" s="2">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="Y86" t="s" s="2">
-        <v>627</v>
+        <v>621</v>
       </c>
       <c r="Z86" t="s" s="2">
-        <v>628</v>
+        <v>622</v>
       </c>
       <c r="AA86" t="s" s="2">
         <v>20</v>
@@ -12427,7 +12399,7 @@
         <v>20</v>
       </c>
       <c r="AF86" t="s" s="2">
-        <v>625</v>
+        <v>619</v>
       </c>
       <c r="AG86" t="s" s="2">
         <v>88</v>
@@ -12442,10 +12414,10 @@
         <v>100</v>
       </c>
       <c r="AK86" t="s" s="2">
-        <v>629</v>
+        <v>623</v>
       </c>
       <c r="AL86" t="s" s="2">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="AM86" t="s" s="2">
         <v>20</v>

</xml_diff>